<commit_message>
added some rf comps
</commit_message>
<xml_diff>
--- a/library/rf.xlsx
+++ b/library/rf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\elem_altium_db2\library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A24684-DA51-42B8-B531-D60C10221358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{556416E7-B0EA-44D5-921B-B6EC99317335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6840" yWindow="1935" windowWidth="21585" windowHeight="11775" xr2:uid="{EE2E7F00-6B54-4C0B-98D7-835E87062BAF}"/>
+    <workbookView xWindow="6285" yWindow="2640" windowWidth="21585" windowHeight="11775" xr2:uid="{EE2E7F00-6B54-4C0B-98D7-835E87062BAF}"/>
   </bookViews>
   <sheets>
     <sheet name="ADC" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="34">
   <si>
     <t>Part Number</t>
   </si>
@@ -88,13 +88,61 @@
   </si>
   <si>
     <t>HMC717ALP3E 16-QFN (3X3)</t>
+  </si>
+  <si>
+    <t>32-QFN (5x5)</t>
+  </si>
+  <si>
+    <t>ADF4355-3BCPZ</t>
+  </si>
+  <si>
+    <t>ADF4355-3BCPZ 32-QFN (5x5)</t>
+  </si>
+  <si>
+    <t>ADF5356</t>
+  </si>
+  <si>
+    <t>ADF5356 32-QFN (5x5)</t>
+  </si>
+  <si>
+    <t>8-MSOP-EP</t>
+  </si>
+  <si>
+    <t>HMC220B</t>
+  </si>
+  <si>
+    <t>HMC220B 8-MSOP-EP</t>
+  </si>
+  <si>
+    <t>HMC369LP3</t>
+  </si>
+  <si>
+    <t>HMC369LP3 16-QFN (3X3)</t>
+  </si>
+  <si>
+    <t>HMC451LP3</t>
+  </si>
+  <si>
+    <t>HMC451LP3 16-QFN (3X3)</t>
+  </si>
+  <si>
+    <t>12-QFN (3Х3)</t>
+  </si>
+  <si>
+    <t>MTX2-73+</t>
+  </si>
+  <si>
+    <t>MTX2-73+ 12-QFN (3Х3)</t>
+  </si>
+  <si>
+    <t>Mimi-Circuits</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,6 +157,14 @@
       <color indexed="8"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -138,10 +194,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent 3 2" xfId="1" xr:uid="{07D6D35A-A25D-4183-ACA2-756DA14CBAEA}"/>
@@ -457,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67671D6E-5D55-4C0C-9FE7-A86F937C6875}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,7 +529,7 @@
     <col min="5" max="6" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -498,7 +555,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -521,7 +578,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -544,7 +601,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -567,7 +624,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
@@ -590,14 +647,147 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="G8" s="2"/>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added some rf components
</commit_message>
<xml_diff>
--- a/library/rf.xlsx
+++ b/library/rf.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitProjects\elem_altium_db2\library\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\elem_altium_db2\library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522FACC9-0A91-4BDF-A722-B5FD55CEA224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068D64D9-5BC7-4B53-97FC-7B87626D8C97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE2E7F00-6B54-4C0B-98D7-835E87062BAF}"/>
+    <workbookView xWindow="6060" yWindow="3735" windowWidth="21585" windowHeight="11775" xr2:uid="{EE2E7F00-6B54-4C0B-98D7-835E87062BAF}"/>
   </bookViews>
   <sheets>
-    <sheet name="ADC" sheetId="1" r:id="rId1"/>
+    <sheet name="rf" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="46">
   <si>
     <t>Part Number</t>
   </si>
@@ -136,6 +136,42 @@
   </si>
   <si>
     <t>Mimi-Circuits</t>
+  </si>
+  <si>
+    <t>CD636</t>
+  </si>
+  <si>
+    <t>ADE-1+</t>
+  </si>
+  <si>
+    <t>ADE-1+ CD636</t>
+  </si>
+  <si>
+    <t>6-TDFN</t>
+  </si>
+  <si>
+    <t>MAAM-011206</t>
+  </si>
+  <si>
+    <t>MAAM-011206 6-TDFN</t>
+  </si>
+  <si>
+    <t>MACOM</t>
+  </si>
+  <si>
+    <t>MADL-011023-14150T</t>
+  </si>
+  <si>
+    <t>MADL-011023-14150T 6-TDFN</t>
+  </si>
+  <si>
+    <t>PL-264</t>
+  </si>
+  <si>
+    <t>NCS2-622+</t>
+  </si>
+  <si>
+    <t>NCS2-622+ PL-264</t>
   </si>
 </sst>
 </file>
@@ -514,19 +550,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67671D6E-5D55-4C0C-9FE7-A86F937C6875}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD34"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
     <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="3" max="3" width="26.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" customWidth="1"/>
-    <col min="5" max="6" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -786,6 +823,121 @@
         <v>33</v>
       </c>
     </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" t="s">
+        <v>43</v>
+      </c>
+      <c r="G16" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>